<commit_message>
Final fixes to BOM
Final fixes to BOM made.
Also started laying out board.
</commit_message>
<xml_diff>
--- a/CatchTheLightV2.xlsx
+++ b/CatchTheLightV2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\ECE388_CatchTheLightV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{2044A8AB-4FA8-4348-AFED-FA4FE04EFD10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C62688-3FC0-4328-A899-80C878EC62C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$J$11</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="102">
   <si>
     <t>Qty</t>
   </si>
@@ -61,18 +60,6 @@
     <t/>
   </si>
   <si>
-    <t>BUTTON_PASSIVE12MM</t>
-  </si>
-  <si>
-    <t>BUTTON_PASSIVE_12MM</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>Button, Passive Capacitive/Touch Sensing Type</t>
-  </si>
-  <si>
     <t>TS-1102S-C-A-B</t>
   </si>
   <si>
@@ -353,6 +340,9 @@
   </si>
   <si>
     <t>U$3</t>
+  </si>
+  <si>
+    <t>http://www.reekart.com/products/30-Surface-Mount-Precision-Metal-Stamping-CR2032-Coin-Cell-Battery-Holder-For-MPD-BC-2003-Replacment.html</t>
   </si>
 </sst>
 </file>
@@ -698,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B71F7FE-3F57-4414-A304-E882D02B622A}">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,10 +730,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -752,34 +742,34 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>50</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>51</v>
       </c>
-      <c r="L1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>54</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>55</v>
       </c>
-      <c r="P1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>59</v>
-      </c>
       <c r="R1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -787,13 +777,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2">
         <v>0.05</v>
@@ -802,10 +792,10 @@
         <v>0.125</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>6</v>
@@ -820,10 +810,10 @@
         <v>5.4100000000000003E-4</v>
       </c>
       <c r="M2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -835,13 +825,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
         <v>0.05</v>
@@ -850,10 +840,10 @@
         <v>0.125</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>6</v>
@@ -868,10 +858,10 @@
         <v>6.5499999999999998E-4</v>
       </c>
       <c r="M3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -883,23 +873,23 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2">
         <v>0.05</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>6</v>
@@ -914,10 +904,10 @@
         <v>5.5459999999999997E-3</v>
       </c>
       <c r="M4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -929,13 +919,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2">
         <v>0.05</v>
@@ -944,10 +934,10 @@
         <v>0.125</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>6</v>
@@ -962,10 +952,10 @@
         <v>1.1130000000000001E-3</v>
       </c>
       <c r="M5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -978,15 +968,15 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>6</v>
@@ -1005,7 +995,7 @@
         <v>1.33</v>
       </c>
       <c r="P6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -1015,21 +1005,21 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>6</v>
@@ -1044,10 +1034,10 @@
         <v>4.0591000000000002E-2</v>
       </c>
       <c r="M7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -1059,21 +1049,21 @@
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>6</v>
@@ -1088,10 +1078,10 @@
         <v>9.417E-3</v>
       </c>
       <c r="M8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -1103,22 +1093,22 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="Q9" s="1">
         <v>0.1162</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1127,18 +1117,18 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>6</v>
@@ -1153,10 +1143,10 @@
         <v>2.8684999999999999E-2</v>
       </c>
       <c r="M10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -1171,18 +1161,18 @@
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>6</v>
@@ -1197,10 +1187,10 @@
         <v>1.1821E-2</v>
       </c>
       <c r="M11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -1213,18 +1203,18 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>6</v>
@@ -1236,31 +1226,29 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
+      <c r="R12" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>6</v>
@@ -1277,40 +1265,11 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-    </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E17" s="2"/>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E19" s="2"/>
@@ -1318,14 +1277,11 @@
     <row r="20" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E21" s="2"/>
+    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N23" s="4"/>
     </row>
     <row r="24" spans="5:14" x14ac:dyDescent="0.25">
       <c r="N24" s="4"/>
-    </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="N25" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1368,10 +1324,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1380,40 +1336,40 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>50</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>51</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>52</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>53</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>54</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>55</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>56</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>57</v>
-      </c>
-      <c r="R1" t="s">
-        <v>58</v>
-      </c>
-      <c r="S1" t="s">
-        <v>59</v>
-      </c>
-      <c r="T1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1424,31 +1380,31 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2">
         <v>0.01</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K2">
         <v>7.4200000000000004E-4</v>
       </c>
       <c r="M2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="N2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -1456,34 +1412,34 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
         <v>0.01</v>
       </c>
       <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
         <v>61</v>
       </c>
-      <c r="G3" t="s">
-        <v>65</v>
-      </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K3">
         <v>9.5200000000000005E-4</v>
       </c>
       <c r="M3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="N3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1491,31 +1447,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2">
         <v>0.01</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K4">
         <v>5.9569999999999996E-3</v>
       </c>
       <c r="M4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="N4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1526,31 +1482,31 @@
         <v>220</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2">
         <v>0.01</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K5">
         <v>2.8E-3</v>
       </c>
       <c r="M5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="N5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1558,34 +1514,34 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2">
         <v>0.01</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K6">
         <v>1.5E-3</v>
       </c>
       <c r="M6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="N6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1596,31 +1552,31 @@
         <v>330</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2">
         <v>0.01</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K7">
         <v>1.5E-3</v>
       </c>
       <c r="M7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="N7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1628,16 +1584,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="O8">
         <v>1.33</v>
@@ -1646,7 +1602,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="R8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -1654,19 +1610,19 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O9">
         <v>0.28999999999999998</v>
@@ -1675,7 +1631,7 @@
         <v>0.24</v>
       </c>
       <c r="R9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -1683,28 +1639,28 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
         <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" t="s">
-        <v>37</v>
       </c>
       <c r="K10">
         <v>0.02</v>
       </c>
       <c r="M10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1712,28 +1668,28 @@
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K11">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="M11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="N11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -1741,22 +1697,22 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="S12">
         <v>0.1162</v>
       </c>
       <c r="T12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>